<commit_message>
rozjazdy aktualne na 14.01
</commit_message>
<xml_diff>
--- a/rozliczenie zbiorcze.xlsx
+++ b/rozliczenie zbiorcze.xlsx
@@ -5,23 +5,24 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\Desktop\KOKSZTYS\Styczeń\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KOKSZTYS\styczeń\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="10905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10910" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Pakiet_Zlecen_WTA_2019_01_03s.s" sheetId="1" r:id="rId1"/>
     <sheet name="rozjazdy 08.01" sheetId="2" r:id="rId2"/>
     <sheet name="rozjazdy 09.01" sheetId="3" r:id="rId3"/>
+    <sheet name="rozjazdy 14.01" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="199">
   <si>
     <t>MONIKA ŁUCZAK</t>
   </si>
@@ -606,12 +607,45 @@
   <si>
     <t>wykonano 10.01.2019</t>
   </si>
+  <si>
+    <t>53-143</t>
+  </si>
+  <si>
+    <t>WROCŁAW, ORLA 26/2 </t>
+  </si>
+  <si>
+    <t>53-416</t>
+  </si>
+  <si>
+    <t>WROCŁAW,ZAPOROSKA 62/14 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARFENOV IEVGENII </t>
+  </si>
+  <si>
+    <t>0005983819</t>
+  </si>
+  <si>
+    <t>0005532869</t>
+  </si>
+  <si>
+    <t>0003961139</t>
+  </si>
+  <si>
+    <t>po 18</t>
+  </si>
+  <si>
+    <t>????</t>
+  </si>
+  <si>
+    <t>?????</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -795,6 +829,14 @@
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1153,7 +1195,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1233,12 +1275,6 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1251,6 +1287,34 @@
     <xf numFmtId="16" fontId="6" fillId="2" borderId="0" xfId="6" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="8" fillId="4" borderId="0" xfId="8" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="7" fillId="3" borderId="0" xfId="7" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% — akcent 1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1572,24 +1636,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O46"/>
+  <dimension ref="A1:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="O36" sqref="O36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1796875" customWidth="1"/>
+    <col min="6" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>184</v>
       </c>
@@ -1606,14 +1670,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>78</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="33" t="s">
         <v>81</v>
       </c>
       <c r="E2" s="2"/>
@@ -1625,15 +1689,15 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A3" s="32" t="s">
         <v>79</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="33" t="s">
         <v>83</v>
       </c>
       <c r="F3" s="3"/>
@@ -1643,18 +1707,18 @@
       <c r="H3" s="8">
         <v>65</v>
       </c>
-      <c r="N3" s="37" t="s">
+      <c r="N3" s="35" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A4" s="32" t="s">
         <v>84</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="33" t="s">
         <v>85</v>
       </c>
       <c r="F4" s="3"/>
@@ -1664,18 +1728,18 @@
       <c r="H4" s="8">
         <v>65</v>
       </c>
-      <c r="N4" s="38" t="s">
+      <c r="N4" s="36" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" s="32" t="s">
         <v>86</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="33" t="s">
         <v>85</v>
       </c>
       <c r="F5" s="3"/>
@@ -1685,18 +1749,18 @@
       <c r="H5" s="8">
         <v>65</v>
       </c>
-      <c r="N5" s="36" t="s">
+      <c r="N5" s="34" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>89</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="33" t="s">
         <v>88</v>
       </c>
       <c r="E6" s="3"/>
@@ -1708,7 +1772,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="27" t="s">
         <v>134</v>
       </c>
@@ -1728,7 +1792,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="27" t="s">
         <v>139</v>
       </c>
@@ -1747,7 +1811,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="27" t="s">
         <v>145</v>
       </c>
@@ -1766,7 +1830,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="27" t="s">
         <v>142</v>
       </c>
@@ -1785,7 +1849,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="27" t="s">
         <v>148</v>
       </c>
@@ -1805,7 +1869,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="27" t="s">
         <v>134</v>
       </c>
@@ -1824,493 +1888,496 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A13" s="27" t="s">
+        <v>195</v>
+      </c>
+      <c r="B13" s="26"/>
+      <c r="C13" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>189</v>
+      </c>
       <c r="E13" s="3"/>
       <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
+      <c r="G13" t="s">
+        <v>82</v>
+      </c>
+      <c r="H13">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A14" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="B14" s="26"/>
+      <c r="C14" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="2"/>
+      <c r="G14" t="s">
+        <v>82</v>
+      </c>
+      <c r="H14">
+        <v>35</v>
+      </c>
+      <c r="I14" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A15" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="2"/>
+      <c r="G15" t="s">
+        <v>82</v>
+      </c>
+      <c r="H15">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A16" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B16" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C16" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D16" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G16" t="s">
         <v>115</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H16" s="8">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A17" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B17" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C17" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="D15" s="23" t="s">
+      <c r="D17" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G17" t="s">
         <v>115</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H17" s="8">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A18" s="12">
         <v>2652454</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B18" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="33" t="s">
+      <c r="D18" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E18" t="s">
         <v>2</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F18" t="s">
         <v>3</v>
-      </c>
-      <c r="G16" t="s">
-        <v>91</v>
-      </c>
-      <c r="H16" s="5">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="12">
-        <v>2657085</v>
-      </c>
-      <c r="B17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="33" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" t="s">
-        <v>7</v>
-      </c>
-      <c r="G17" t="s">
-        <v>91</v>
-      </c>
-      <c r="H17" s="8">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="12">
-        <v>2663720</v>
-      </c>
-      <c r="B18" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="33" t="s">
-        <v>183</v>
-      </c>
-      <c r="E18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" t="s">
-        <v>11</v>
       </c>
       <c r="G18" t="s">
         <v>91</v>
       </c>
-      <c r="H18" s="8">
+      <c r="H18" s="5">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="12">
+        <v>2657085</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" t="s">
+        <v>91</v>
+      </c>
+      <c r="H19" s="8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A20" s="12">
+        <v>2663720</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" t="s">
+        <v>91</v>
+      </c>
+      <c r="H20" s="8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A21" s="12">
         <v>2949099</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B21" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C21" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="33" t="s">
+      <c r="D21" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E21" t="s">
         <v>14</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F21" t="s">
         <v>15</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G21" t="s">
         <v>94</v>
-      </c>
-      <c r="H19" s="5">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="12">
-        <v>2958822</v>
-      </c>
-      <c r="B20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="E20" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G20" t="s">
-        <v>96</v>
-      </c>
-      <c r="H20" s="25">
-        <v>70</v>
-      </c>
-      <c r="J20" t="s">
-        <v>97</v>
-      </c>
-      <c r="K20" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="12">
-        <v>3037547</v>
-      </c>
-      <c r="B21" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="E21">
-        <v>8382958</v>
-      </c>
-      <c r="F21" t="s">
-        <v>22</v>
-      </c>
-      <c r="G21" t="s">
-        <v>99</v>
       </c>
       <c r="H21" s="5">
         <v>40</v>
       </c>
-      <c r="J21" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="12">
-        <v>3067160</v>
+        <v>2958822</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>25</v>
+        <v>17</v>
+      </c>
+      <c r="D22" s="31" t="s">
+        <v>95</v>
       </c>
       <c r="E22" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="F22" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="G22" t="s">
-        <v>99</v>
-      </c>
-      <c r="H22" s="5">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="H22" s="25">
+        <v>70</v>
+      </c>
+      <c r="J22" t="s">
+        <v>97</v>
+      </c>
+      <c r="K22" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="12">
-        <v>3073191</v>
+        <v>3037547</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E23" t="s">
-        <v>31</v>
+        <v>21</v>
+      </c>
+      <c r="D23" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="E23">
+        <v>8382958</v>
       </c>
       <c r="F23" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="G23" t="s">
         <v>99</v>
       </c>
       <c r="H23" s="5">
+        <v>40</v>
+      </c>
+      <c r="J23" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A24" s="12">
+        <v>3067160</v>
+      </c>
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" t="s">
+        <v>27</v>
+      </c>
+      <c r="G24" t="s">
+        <v>99</v>
+      </c>
+      <c r="H24" s="5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A25" s="12">
+        <v>3073191</v>
+      </c>
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" t="s">
+        <v>32</v>
+      </c>
+      <c r="G25" t="s">
+        <v>99</v>
+      </c>
+      <c r="H25" s="5">
         <v>70</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J25" t="s">
         <v>101</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K25" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="28">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A26" s="28">
         <v>3074967</v>
       </c>
-      <c r="B24" s="28" t="s">
+      <c r="B26" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="29" t="s">
+      <c r="C26" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="30" t="s">
+      <c r="D26" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="E24" s="28">
+      <c r="E26" s="28">
         <v>1755131</v>
       </c>
-      <c r="F24" s="28" t="s">
+      <c r="F26" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="G24" s="28" t="s">
+      <c r="G26" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="H24" s="28" t="s">
+      <c r="H26" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="I24" s="28"/>
-      <c r="J24" s="28" t="s">
+      <c r="I26" s="28"/>
+      <c r="J26" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="K24" s="28">
+      <c r="K26" s="28">
         <v>104</v>
       </c>
-      <c r="L24" s="28"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="12">
+      <c r="L26" s="28"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A27" s="12">
         <v>2955619</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B27" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D25" s="33" t="s">
+      <c r="D27" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E25">
+      <c r="E27">
         <v>2181000</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F27" t="s">
         <v>38</v>
-      </c>
-      <c r="G25" t="s">
-        <v>96</v>
-      </c>
-      <c r="H25" s="8">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="12">
-        <v>3037067</v>
-      </c>
-      <c r="B26" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="E26">
-        <v>3458347</v>
-      </c>
-      <c r="F26" t="s">
-        <v>42</v>
-      </c>
-      <c r="G26" t="s">
-        <v>99</v>
-      </c>
-      <c r="H26" s="8">
-        <v>70</v>
-      </c>
-      <c r="J26" t="s">
-        <v>105</v>
-      </c>
-      <c r="K26">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="12">
-        <v>2951874</v>
-      </c>
-      <c r="B27" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="E27" t="s">
-        <v>45</v>
-      </c>
-      <c r="F27" t="s">
-        <v>46</v>
       </c>
       <c r="G27" t="s">
         <v>96</v>
       </c>
-      <c r="H27" s="25">
+      <c r="H27" s="8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A28" s="12">
+        <v>3037067</v>
+      </c>
+      <c r="B28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E28">
+        <v>3458347</v>
+      </c>
+      <c r="F28" t="s">
+        <v>42</v>
+      </c>
+      <c r="G28" t="s">
+        <v>99</v>
+      </c>
+      <c r="H28" s="8">
         <v>70</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="12">
+      <c r="J28" t="s">
+        <v>105</v>
+      </c>
+      <c r="K28">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A29" s="12">
+        <v>2951874</v>
+      </c>
+      <c r="B29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E29" t="s">
+        <v>45</v>
+      </c>
+      <c r="F29" t="s">
+        <v>46</v>
+      </c>
+      <c r="G29" t="s">
+        <v>96</v>
+      </c>
+      <c r="H29" s="25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A30" s="12">
         <v>2966414</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B30" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C30" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D30" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="E28">
+      <c r="E30">
         <v>3628938</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F30" t="s">
         <v>49</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G30" t="s">
         <v>96</v>
       </c>
-      <c r="H28" s="25">
+      <c r="H30" s="25">
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A31" s="12">
         <v>3266106</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B31" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C31" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="D31" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="E29">
+      <c r="E31">
         <v>3211863</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F31" t="s">
         <v>53</v>
-      </c>
-      <c r="G29" t="s">
-        <v>106</v>
-      </c>
-      <c r="H29" s="5">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="12">
-        <v>3266289</v>
-      </c>
-      <c r="B30" t="s">
-        <v>54</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E30">
-        <v>1929525</v>
-      </c>
-      <c r="F30" t="s">
-        <v>57</v>
-      </c>
-      <c r="G30" t="s">
-        <v>106</v>
-      </c>
-      <c r="H30" s="8">
-        <v>65</v>
-      </c>
-      <c r="K30" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="12">
-        <v>3266324</v>
-      </c>
-      <c r="B31" t="s">
-        <v>58</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="E31">
-        <v>1603687</v>
-      </c>
-      <c r="F31" t="s">
-        <v>61</v>
       </c>
       <c r="G31" t="s">
         <v>106</v>
@@ -2319,21 +2386,24 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="12">
-        <v>3266133</v>
+        <v>3266289</v>
       </c>
       <c r="B32" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>63</v>
+        <v>56</v>
+      </c>
+      <c r="E32">
+        <v>1929525</v>
       </c>
       <c r="F32" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="G32" t="s">
         <v>106</v>
@@ -2341,68 +2411,74 @@
       <c r="H32" s="8">
         <v>65</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K32" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33" s="12">
-        <v>3265971</v>
+        <v>3266324</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D33" s="33" t="s">
-        <v>107</v>
+        <v>59</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E33">
+        <v>1603687</v>
       </c>
       <c r="F33" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G33" t="s">
         <v>106</v>
       </c>
       <c r="H33" s="5">
-        <v>32.5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34" s="12">
-        <v>3266023</v>
+        <v>3266133</v>
       </c>
       <c r="B34" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D34" s="33" t="s">
-        <v>107</v>
+        <v>9</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>63</v>
       </c>
       <c r="F34" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G34" t="s">
         <v>106</v>
       </c>
-      <c r="H34" s="5">
-        <v>32.5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H34" s="8">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A35" s="12">
-        <v>3266265</v>
+        <v>3265971</v>
       </c>
       <c r="B35" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>70</v>
+        <v>24</v>
+      </c>
+      <c r="D35" s="31" t="s">
+        <v>107</v>
       </c>
       <c r="F35" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G35" t="s">
         <v>106</v>
@@ -2411,21 +2487,21 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A36" s="12">
-        <v>3266180</v>
+        <v>3266023</v>
       </c>
       <c r="B36" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>70</v>
+        <v>24</v>
+      </c>
+      <c r="D36" s="31" t="s">
+        <v>107</v>
       </c>
       <c r="F36" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G36" t="s">
         <v>106</v>
@@ -2434,187 +2510,178 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="28">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A37" s="12">
+        <v>3266265</v>
+      </c>
+      <c r="B37" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="F37" t="s">
+        <v>71</v>
+      </c>
+      <c r="G37" t="s">
+        <v>106</v>
+      </c>
+      <c r="H37" s="5">
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A38" s="12">
+        <v>3266180</v>
+      </c>
+      <c r="B38" t="s">
+        <v>68</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="F38" t="s">
+        <v>72</v>
+      </c>
+      <c r="G38" t="s">
+        <v>106</v>
+      </c>
+      <c r="H38" s="5">
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A39" s="28">
         <v>3266321</v>
       </c>
-      <c r="B37" s="28" t="s">
+      <c r="B39" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="C37" s="28" t="s">
+      <c r="C39" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="D37" s="28" t="s">
+      <c r="D39" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="E37" s="28"/>
-      <c r="F37" s="28" t="s">
+      <c r="E39" s="28"/>
+      <c r="F39" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G37" s="28" t="s">
+      <c r="G39" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="H37" s="28" t="s">
+      <c r="H39" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="I37" s="28"/>
-      <c r="J37" s="28"/>
-      <c r="K37" s="28"/>
-      <c r="L37" s="28"/>
-      <c r="M37" s="28"/>
-      <c r="N37" s="28"/>
-      <c r="O37" s="28"/>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="28">
+      <c r="I39" s="28"/>
+      <c r="J39" s="28"/>
+      <c r="K39" s="28"/>
+      <c r="L39" s="28"/>
+      <c r="M39" s="28"/>
+      <c r="N39" s="28"/>
+      <c r="O39" s="28"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A40" s="28">
         <v>3265990</v>
       </c>
-      <c r="B38" s="28" t="s">
+      <c r="B40" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="C38" s="28" t="s">
+      <c r="C40" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="D38" s="28" t="s">
+      <c r="D40" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="E38" s="28"/>
-      <c r="F38" s="28" t="s">
+      <c r="E40" s="28"/>
+      <c r="F40" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="G38" s="28" t="s">
+      <c r="G40" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="H38" s="28" t="s">
+      <c r="H40" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="I38" s="28"/>
-      <c r="J38" s="28"/>
-      <c r="K38" s="28"/>
-      <c r="L38" s="28"/>
-      <c r="M38" s="28"/>
-      <c r="N38" s="28"/>
-      <c r="O38" s="28"/>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39">
+      <c r="I40" s="28"/>
+      <c r="J40" s="28"/>
+      <c r="K40" s="28"/>
+      <c r="L40" s="28"/>
+      <c r="M40" s="28"/>
+      <c r="N40" s="28"/>
+      <c r="O40" s="28"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A41">
         <v>3274450</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B41" t="s">
         <v>151</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C41" t="s">
         <v>152</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D41" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F41" t="s">
         <v>154</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G41" t="s">
         <v>106</v>
       </c>
-      <c r="H39">
+      <c r="H41">
         <v>90</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A42">
         <v>3274740</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B42" t="s">
         <v>155</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C42" t="s">
         <v>152</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D42" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F42" t="s">
         <v>157</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G42" t="s">
         <v>106</v>
       </c>
-      <c r="H40">
+      <c r="H42">
         <v>90</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A43">
         <v>2961585</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B43" t="s">
         <v>158</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C43" t="s">
         <v>159</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D43" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E43" t="s">
         <v>161</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F43" t="s">
         <v>162</v>
-      </c>
-      <c r="G41" t="s">
-        <v>96</v>
-      </c>
-      <c r="H41">
-        <v>70</v>
-      </c>
-      <c r="J41" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>2962452</v>
-      </c>
-      <c r="B42" t="s">
-        <v>158</v>
-      </c>
-      <c r="C42" t="s">
-        <v>159</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="E42" t="s">
-        <v>161</v>
-      </c>
-      <c r="F42" t="s">
-        <v>163</v>
-      </c>
-      <c r="G42" t="s">
-        <v>96</v>
-      </c>
-      <c r="H42">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>2966808</v>
-      </c>
-      <c r="B43" t="s">
-        <v>164</v>
-      </c>
-      <c r="C43" t="s">
-        <v>165</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="E43">
-        <v>9176943</v>
-      </c>
-      <c r="F43" t="s">
-        <v>167</v>
       </c>
       <c r="G43" t="s">
         <v>96</v>
@@ -2622,88 +2689,149 @@
       <c r="H43">
         <v>70</v>
       </c>
-      <c r="J43">
+      <c r="I43" s="37" t="s">
+        <v>197</v>
+      </c>
+      <c r="J43" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>2962452</v>
+      </c>
+      <c r="B44" t="s">
+        <v>158</v>
+      </c>
+      <c r="C44" t="s">
+        <v>159</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E44" t="s">
+        <v>161</v>
+      </c>
+      <c r="F44" t="s">
+        <v>163</v>
+      </c>
+      <c r="G44" t="s">
+        <v>96</v>
+      </c>
+      <c r="H44">
+        <v>70</v>
+      </c>
+      <c r="I44" s="37" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>2966808</v>
+      </c>
+      <c r="B45" t="s">
+        <v>164</v>
+      </c>
+      <c r="C45" t="s">
+        <v>165</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="E45">
+        <v>9176943</v>
+      </c>
+      <c r="F45" t="s">
+        <v>167</v>
+      </c>
+      <c r="G45" t="s">
+        <v>96</v>
+      </c>
+      <c r="H45">
+        <v>70</v>
+      </c>
+      <c r="J45">
         <v>51</v>
       </c>
-      <c r="K43" t="s">
+      <c r="K45" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A44">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A46">
         <v>3274419</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B46" t="s">
         <v>168</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C46" t="s">
         <v>169</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D46" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F46" t="s">
         <v>171</v>
-      </c>
-      <c r="G44" t="s">
-        <v>106</v>
-      </c>
-      <c r="H44">
-        <v>90</v>
-      </c>
-      <c r="J44">
-        <v>58</v>
-      </c>
-      <c r="K44" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>3274597</v>
-      </c>
-      <c r="B45" t="s">
-        <v>172</v>
-      </c>
-      <c r="C45" t="s">
-        <v>173</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="F45" t="s">
-        <v>175</v>
-      </c>
-      <c r="G45" t="s">
-        <v>106</v>
-      </c>
-      <c r="H45">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>3274543</v>
-      </c>
-      <c r="B46" t="s">
-        <v>176</v>
-      </c>
-      <c r="C46" t="s">
-        <v>165</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="F46" t="s">
-        <v>178</v>
       </c>
       <c r="G46" t="s">
         <v>106</v>
       </c>
       <c r="H46">
+        <v>90</v>
+      </c>
+      <c r="J46">
+        <v>58</v>
+      </c>
+      <c r="K46" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>3274597</v>
+      </c>
+      <c r="B47" t="s">
+        <v>172</v>
+      </c>
+      <c r="C47" t="s">
+        <v>173</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="F47" t="s">
+        <v>175</v>
+      </c>
+      <c r="G47" t="s">
+        <v>106</v>
+      </c>
+      <c r="H47">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>3274543</v>
+      </c>
+      <c r="B48" t="s">
+        <v>176</v>
+      </c>
+      <c r="C48" t="s">
+        <v>165</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="F48" t="s">
+        <v>178</v>
+      </c>
+      <c r="G48" t="s">
+        <v>106</v>
+      </c>
+      <c r="H48">
         <v>65</v>
       </c>
-      <c r="J46" t="s">
+      <c r="J48" t="s">
         <v>182</v>
       </c>
     </row>
@@ -2718,18 +2846,18 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A26"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" style="12" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="10.453125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="17.81640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.81640625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="25.26953125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11">
         <v>2663720</v>
       </c>
@@ -2755,7 +2883,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -2763,7 +2891,7 @@
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="11">
         <v>3037547</v>
       </c>
@@ -2792,7 +2920,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -2800,7 +2928,7 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11">
         <v>3067160</v>
       </c>
@@ -2826,7 +2954,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -2834,7 +2962,7 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11">
         <v>3265971</v>
       </c>
@@ -2858,7 +2986,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="11">
         <v>3266023</v>
       </c>
@@ -2882,7 +3010,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -2890,7 +3018,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11">
         <v>2949099</v>
       </c>
@@ -2916,7 +3044,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="11"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
@@ -2924,7 +3052,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="11">
         <v>2652454</v>
       </c>
@@ -2950,7 +3078,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -2958,7 +3086,7 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="11">
         <v>3266321</v>
       </c>
@@ -2988,7 +3116,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="11">
         <v>3265990</v>
       </c>
@@ -3012,7 +3140,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
@@ -3020,7 +3148,7 @@
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
     </row>
-    <row r="17" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="11">
         <v>3073191</v>
       </c>
@@ -3052,7 +3180,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="11"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
@@ -3060,7 +3188,7 @@
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
     </row>
-    <row r="19" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="11">
         <v>3266265</v>
       </c>
@@ -3084,7 +3212,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="11">
         <v>3266180</v>
       </c>
@@ -3108,7 +3236,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="11"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -3116,7 +3244,7 @@
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
     </row>
-    <row r="22" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="11">
         <v>3266324</v>
       </c>
@@ -3142,7 +3270,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="11"/>
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
@@ -3150,7 +3278,7 @@
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
     </row>
-    <row r="24" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="11" t="s">
         <v>78</v>
       </c>
@@ -3170,7 +3298,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="11"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -3178,7 +3306,7 @@
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
     </row>
-    <row r="26" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="11">
         <v>3266106</v>
       </c>
@@ -3214,23 +3342,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection sqref="A1:D2"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" style="12" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" style="10" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" style="12" customWidth="1"/>
+    <col min="2" max="2" width="22.26953125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="6.54296875" style="12" customWidth="1"/>
+    <col min="4" max="4" width="26.7265625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="38" t="s">
         <v>127</v>
       </c>
       <c r="C1" s="11" t="s">
@@ -3248,9 +3376,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32"/>
-      <c r="B2" s="31"/>
+    <row r="2" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="39"/>
+      <c r="B2" s="38"/>
       <c r="C2" s="11" t="s">
         <v>126</v>
       </c>
@@ -3260,7 +3388,7 @@
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
         <v>79</v>
       </c>
@@ -3280,7 +3408,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -3288,7 +3416,7 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11">
         <v>3266133</v>
       </c>
@@ -3312,7 +3440,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -3320,7 +3448,7 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
         <v>84</v>
       </c>
@@ -3340,7 +3468,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
         <v>86</v>
       </c>
@@ -3360,7 +3488,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -3368,7 +3496,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11">
         <v>2955619</v>
       </c>
@@ -3394,7 +3522,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="11"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
@@ -3402,7 +3530,7 @@
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="11">
         <v>3266289</v>
       </c>
@@ -3431,7 +3559,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -3439,7 +3567,7 @@
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="11">
         <v>2657085</v>
       </c>
@@ -3465,7 +3593,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="11"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -3473,7 +3601,7 @@
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="11">
         <v>3037067</v>
       </c>
@@ -3505,7 +3633,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -3513,7 +3641,7 @@
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
     </row>
-    <row r="18" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="13" t="s">
         <v>89</v>
       </c>
@@ -3533,7 +3661,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="11"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -3541,7 +3669,7 @@
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
     </row>
-    <row r="20" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="11">
         <v>2958822</v>
       </c>
@@ -3573,7 +3701,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="11"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -3581,7 +3709,7 @@
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
     </row>
-    <row r="22" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="11">
         <v>2951874</v>
       </c>
@@ -3607,7 +3735,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="11">
         <v>2966414</v>
       </c>
@@ -3633,7 +3761,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="11"/>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
@@ -3641,7 +3769,7 @@
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
     </row>
-    <row r="25" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
         <v>116</v>
       </c>
@@ -3660,7 +3788,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="11"/>
       <c r="B26" s="17" t="s">
         <v>122</v>
@@ -3680,7 +3808,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="11"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -3688,7 +3816,7 @@
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
     </row>
-    <row r="28" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
         <v>130</v>
       </c>
@@ -3699,13 +3827,13 @@
       <c r="D28" s="9"/>
       <c r="F28" s="7"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B32"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B33"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B34"/>
     </row>
   </sheetData>
@@ -3716,4 +3844,526 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33" style="41" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" customWidth="1"/>
+    <col min="6" max="6" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7">
+        <v>2966808</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D1" s="46" t="s">
+        <v>166</v>
+      </c>
+      <c r="E1" s="7">
+        <v>9176943</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="G1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="7">
+        <v>3274543</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="G3" t="s">
+        <v>106</v>
+      </c>
+      <c r="H3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="7">
+        <v>3274419</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="G5" t="s">
+        <v>106</v>
+      </c>
+      <c r="H5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="7">
+        <v>3274740</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>156</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="G7" t="s">
+        <v>106</v>
+      </c>
+      <c r="H7">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="7">
+        <v>3274450</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>153</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="G9" t="s">
+        <v>106</v>
+      </c>
+      <c r="H9">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="7">
+        <v>3274597</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>174</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="G11" t="s">
+        <v>106</v>
+      </c>
+      <c r="H11">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="44" t="s">
+        <v>134</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="E13" s="16"/>
+      <c r="F13" s="15"/>
+      <c r="G13" t="s">
+        <v>82</v>
+      </c>
+      <c r="H13">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="B15" s="45"/>
+      <c r="C15" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="E15" s="16"/>
+      <c r="F15" s="15"/>
+      <c r="G15" t="s">
+        <v>82</v>
+      </c>
+      <c r="H15">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="44" t="s">
+        <v>195</v>
+      </c>
+      <c r="B17" s="45"/>
+      <c r="C17" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="E17" s="16"/>
+      <c r="F17" s="15"/>
+      <c r="G17" t="s">
+        <v>82</v>
+      </c>
+      <c r="H17">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="B19" s="45"/>
+      <c r="C19" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="E19" s="16"/>
+      <c r="F19" s="15"/>
+      <c r="G19" t="s">
+        <v>82</v>
+      </c>
+      <c r="H19">
+        <v>35</v>
+      </c>
+      <c r="I19" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="B21" s="45" t="s">
+        <v>192</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="E21" s="16"/>
+      <c r="F21" s="15"/>
+      <c r="G21" t="s">
+        <v>82</v>
+      </c>
+      <c r="H21">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="44" t="s">
+        <v>134</v>
+      </c>
+      <c r="B23" s="45"/>
+      <c r="C23" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="E23" s="16"/>
+      <c r="F23" s="15"/>
+      <c r="G23" t="s">
+        <v>82</v>
+      </c>
+      <c r="H23">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="44" t="s">
+        <v>142</v>
+      </c>
+      <c r="B25" s="7"/>
+      <c r="C25" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="E25" s="16"/>
+      <c r="F25" s="15"/>
+      <c r="G25" t="s">
+        <v>82</v>
+      </c>
+      <c r="H25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="44" t="s">
+        <v>145</v>
+      </c>
+      <c r="B27" s="7"/>
+      <c r="C27" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="E27" s="16"/>
+      <c r="F27" s="15"/>
+      <c r="G27" t="s">
+        <v>82</v>
+      </c>
+      <c r="H27">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="44" t="s">
+        <v>139</v>
+      </c>
+      <c r="B29" s="7"/>
+      <c r="C29" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="E29" s="16"/>
+      <c r="F29" s="15"/>
+      <c r="G29" t="s">
+        <v>82</v>
+      </c>
+      <c r="H29">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>2961585</v>
+      </c>
+      <c r="B35" t="s">
+        <v>158</v>
+      </c>
+      <c r="C35" t="s">
+        <v>159</v>
+      </c>
+      <c r="D35" s="40" t="s">
+        <v>160</v>
+      </c>
+      <c r="E35" t="s">
+        <v>161</v>
+      </c>
+      <c r="F35" t="s">
+        <v>162</v>
+      </c>
+      <c r="G35" t="s">
+        <v>96</v>
+      </c>
+      <c r="H35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>2962452</v>
+      </c>
+      <c r="B36" t="s">
+        <v>158</v>
+      </c>
+      <c r="C36" t="s">
+        <v>159</v>
+      </c>
+      <c r="D36" s="40" t="s">
+        <v>160</v>
+      </c>
+      <c r="E36" t="s">
+        <v>161</v>
+      </c>
+      <c r="F36" t="s">
+        <v>163</v>
+      </c>
+      <c r="G36" t="s">
+        <v>96</v>
+      </c>
+      <c r="H36">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
aktualizacja na 15.01 14:00
</commit_message>
<xml_diff>
--- a/rozliczenie zbiorcze.xlsx
+++ b/rozliczenie zbiorcze.xlsx
@@ -5,24 +5,25 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KOKSZTYS\styczeń\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\Desktop\KOKSZTYS\Styczeń\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10910" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="10905" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Pakiet_Zlecen_WTA_2019_01_03s.s" sheetId="1" r:id="rId1"/>
     <sheet name="rozjazdy 08.01" sheetId="2" r:id="rId2"/>
     <sheet name="rozjazdy 09.01" sheetId="3" r:id="rId3"/>
     <sheet name="rozjazdy 14.01" sheetId="4" r:id="rId4"/>
+    <sheet name="rozjazdy 15.01" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="231">
   <si>
     <t>MONIKA ŁUCZAK</t>
   </si>
@@ -639,6 +640,102 @@
   </si>
   <si>
     <t>?????</t>
+  </si>
+  <si>
+    <t>SOLIDBUD BUDUJ SOLIDNIE STANKIEWICZ MARCIN MARCIN STANKIEWICZ</t>
+  </si>
+  <si>
+    <t>55-036</t>
+  </si>
+  <si>
+    <t>BOCZNA 3, 55-036 SZEWCE</t>
+  </si>
+  <si>
+    <t>1425.84</t>
+  </si>
+  <si>
+    <t>a48</t>
+  </si>
+  <si>
+    <t>ELŻBIETA KAMECKA</t>
+  </si>
+  <si>
+    <t>54-107</t>
+  </si>
+  <si>
+    <t>MAŚLICKA 8C/6 WROCŁAW</t>
+  </si>
+  <si>
+    <t>11565.58</t>
+  </si>
+  <si>
+    <t>bph</t>
+  </si>
+  <si>
+    <t>ZBIGNIEW BAŁAGA</t>
+  </si>
+  <si>
+    <t>50-362</t>
+  </si>
+  <si>
+    <t>MINKOWSKIEGO 10/2 WROCŁAW</t>
+  </si>
+  <si>
+    <t>3113.22</t>
+  </si>
+  <si>
+    <t>JANUSZ QUIRINI</t>
+  </si>
+  <si>
+    <t>53-209</t>
+  </si>
+  <si>
+    <t>ROGOZIŃSKIEGO 18/2 WROCŁAW</t>
+  </si>
+  <si>
+    <t>1686.02</t>
+  </si>
+  <si>
+    <t>PATRYK BIAŁEK</t>
+  </si>
+  <si>
+    <t>54-062</t>
+  </si>
+  <si>
+    <t>STABŁOWICKA 118E/13 WROCŁAW</t>
+  </si>
+  <si>
+    <t>0405817,730405871,</t>
+  </si>
+  <si>
+    <t>3878.03</t>
+  </si>
+  <si>
+    <t>MAŁGORZATA WÓJCIK</t>
+  </si>
+  <si>
+    <t>54-058</t>
+  </si>
+  <si>
+    <t>POMARAŃCZOWA 3, 54-058 WROCŁAW</t>
+  </si>
+  <si>
+    <t>2174.48</t>
+  </si>
+  <si>
+    <t>KATARZYNA BOROWCZYK</t>
+  </si>
+  <si>
+    <t>54-079</t>
+  </si>
+  <si>
+    <t>MAŁOMICKA 18, 54-079 WROCŁAW</t>
+  </si>
+  <si>
+    <t>5352.13</t>
+  </si>
+  <si>
+    <t>wykonano 14.01</t>
   </si>
 </sst>
 </file>
@@ -1020,7 +1117,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1150,6 +1247,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1195,7 +1318,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1287,13 +1410,6 @@
     <xf numFmtId="16" fontId="6" fillId="2" borderId="0" xfId="6" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="8" fillId="4" borderId="0" xfId="8" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="7" fillId="3" borderId="0" xfId="7" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -1315,6 +1431,39 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="9" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="9"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% — akcent 1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1636,24 +1785,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O48"/>
+  <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52:G52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.1796875" customWidth="1"/>
-    <col min="6" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>184</v>
       </c>
@@ -1670,7 +1819,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>78</v>
       </c>
@@ -1689,7 +1838,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
         <v>79</v>
       </c>
@@ -1711,7 +1860,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
         <v>84</v>
       </c>
@@ -1732,7 +1881,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
         <v>86</v>
       </c>
@@ -1753,7 +1902,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>89</v>
       </c>
@@ -1771,8 +1920,11 @@
       <c r="H6" s="25">
         <v>65</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N6" s="48" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
         <v>134</v>
       </c>
@@ -1792,7 +1944,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
         <v>139</v>
       </c>
@@ -1811,7 +1963,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
         <v>145</v>
       </c>
@@ -1830,7 +1982,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
         <v>142</v>
       </c>
@@ -1849,7 +2001,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
         <v>148</v>
       </c>
@@ -1869,7 +2021,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
         <v>134</v>
       </c>
@@ -1888,7 +2040,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
         <v>195</v>
       </c>
@@ -1908,7 +2060,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
         <v>193</v>
       </c>
@@ -1931,7 +2083,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>194</v>
       </c>
@@ -1953,7 +2105,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>123</v>
       </c>
@@ -1973,7 +2125,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>123</v>
       </c>
@@ -1993,7 +2145,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>2652454</v>
       </c>
@@ -2019,7 +2171,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>2657085</v>
       </c>
@@ -2045,7 +2197,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>2663720</v>
       </c>
@@ -2071,7 +2223,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>2949099</v>
       </c>
@@ -2097,7 +2249,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>2958822</v>
       </c>
@@ -2129,7 +2281,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>3037547</v>
       </c>
@@ -2158,7 +2310,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>3067160</v>
       </c>
@@ -2184,7 +2336,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>3073191</v>
       </c>
@@ -2216,7 +2368,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="28">
         <v>3074967</v>
       </c>
@@ -2250,7 +2402,7 @@
       </c>
       <c r="L26" s="28"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>2955619</v>
       </c>
@@ -2276,7 +2428,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <v>3037067</v>
       </c>
@@ -2308,7 +2460,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <v>2951874</v>
       </c>
@@ -2334,7 +2486,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <v>2966414</v>
       </c>
@@ -2360,7 +2512,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <v>3266106</v>
       </c>
@@ -2386,7 +2538,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>3266289</v>
       </c>
@@ -2415,7 +2567,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <v>3266324</v>
       </c>
@@ -2441,7 +2593,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>3266133</v>
       </c>
@@ -2464,7 +2616,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <v>3265971</v>
       </c>
@@ -2487,7 +2639,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
         <v>3266023</v>
       </c>
@@ -2510,7 +2662,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
         <v>3266265</v>
       </c>
@@ -2533,7 +2685,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
         <v>3266180</v>
       </c>
@@ -2556,7 +2708,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="28">
         <v>3266321</v>
       </c>
@@ -2587,7 +2739,7 @@
       <c r="N39" s="28"/>
       <c r="O39" s="28"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="28">
         <v>3265990</v>
       </c>
@@ -2618,221 +2770,423 @@
       <c r="N40" s="28"/>
       <c r="O40" s="28"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A41">
+    <row r="41" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="12">
         <v>3274450</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D41" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G41" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="H41">
+      <c r="H41" s="47">
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A42">
+    <row r="42" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="12">
         <v>3274740</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D42" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="G42" t="s">
+      <c r="G42" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="H42">
+      <c r="H42" s="47">
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A43">
+    <row r="43" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
         <v>2961585</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="4" t="s">
         <v>159</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="G43" t="s">
+      <c r="G43" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="H43">
+      <c r="H43" s="4">
         <v>70</v>
       </c>
-      <c r="I43" s="37" t="s">
+      <c r="I43" s="46" t="s">
         <v>197</v>
       </c>
-      <c r="J43" t="s">
+      <c r="J43" s="4" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A44">
+    <row r="44" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
         <v>2962452</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="4" t="s">
         <v>159</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="G44" t="s">
+      <c r="G44" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="H44">
+      <c r="H44" s="4">
         <v>70</v>
       </c>
-      <c r="I44" s="37" t="s">
+      <c r="I44" s="46" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A45">
+    <row r="45" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="12">
         <v>2966808</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D45" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="12">
         <v>9176943</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F45" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="G45" t="s">
+      <c r="G45" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="H45">
+      <c r="H45" s="47">
         <v>70</v>
       </c>
-      <c r="J45">
+      <c r="J45" s="12">
         <v>51</v>
       </c>
-      <c r="K45" t="s">
+      <c r="K45" s="12" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A46">
+    <row r="46" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="12">
         <v>3274419</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="D46" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F46" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="G46" t="s">
+      <c r="G46" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="H46">
+      <c r="H46" s="47">
         <v>90</v>
       </c>
-      <c r="J46">
+      <c r="J46" s="12">
         <v>58</v>
       </c>
-      <c r="K46" t="s">
+      <c r="K46" s="12" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A47">
+    <row r="47" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="12">
         <v>3274597</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="D47" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F47" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="G47" t="s">
+      <c r="G47" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="H47">
+      <c r="H47" s="47">
         <v>90</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A48">
+    <row r="48" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="12">
         <v>3274543</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D48" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F48" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G48" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="H48">
+      <c r="H48" s="47">
         <v>65</v>
       </c>
-      <c r="J48" t="s">
+      <c r="J48" s="12" t="s">
         <v>182</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>3276446</v>
+      </c>
+      <c r="B49" t="s">
+        <v>199</v>
+      </c>
+      <c r="C49" t="s">
+        <v>200</v>
+      </c>
+      <c r="D49" t="s">
+        <v>201</v>
+      </c>
+      <c r="F49" t="s">
+        <v>202</v>
+      </c>
+      <c r="G49" t="s">
+        <v>203</v>
+      </c>
+      <c r="H49" s="49">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>3268518</v>
+      </c>
+      <c r="B50" t="s">
+        <v>204</v>
+      </c>
+      <c r="C50" t="s">
+        <v>205</v>
+      </c>
+      <c r="D50" t="s">
+        <v>206</v>
+      </c>
+      <c r="E50">
+        <v>4329093</v>
+      </c>
+      <c r="F50" t="s">
+        <v>207</v>
+      </c>
+      <c r="G50" t="s">
+        <v>208</v>
+      </c>
+      <c r="H50" s="49">
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>3268531</v>
+      </c>
+      <c r="B51" t="s">
+        <v>209</v>
+      </c>
+      <c r="C51" t="s">
+        <v>210</v>
+      </c>
+      <c r="D51" t="s">
+        <v>211</v>
+      </c>
+      <c r="E51">
+        <v>6484</v>
+      </c>
+      <c r="F51" t="s">
+        <v>212</v>
+      </c>
+      <c r="G51" t="s">
+        <v>208</v>
+      </c>
+      <c r="H51" s="49">
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>3268534</v>
+      </c>
+      <c r="B52" t="s">
+        <v>213</v>
+      </c>
+      <c r="C52" t="s">
+        <v>214</v>
+      </c>
+      <c r="D52" t="s">
+        <v>215</v>
+      </c>
+      <c r="E52">
+        <v>1862974</v>
+      </c>
+      <c r="F52" t="s">
+        <v>216</v>
+      </c>
+      <c r="G52" t="s">
+        <v>208</v>
+      </c>
+      <c r="H52" s="49">
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>3276430</v>
+      </c>
+      <c r="B53" t="s">
+        <v>217</v>
+      </c>
+      <c r="C53" t="s">
+        <v>218</v>
+      </c>
+      <c r="D53" t="s">
+        <v>219</v>
+      </c>
+      <c r="E53" t="s">
+        <v>220</v>
+      </c>
+      <c r="F53" t="s">
+        <v>221</v>
+      </c>
+      <c r="G53" t="s">
+        <v>208</v>
+      </c>
+      <c r="H53" s="49">
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>3276426</v>
+      </c>
+      <c r="B54" t="s">
+        <v>222</v>
+      </c>
+      <c r="C54" t="s">
+        <v>223</v>
+      </c>
+      <c r="D54" t="s">
+        <v>224</v>
+      </c>
+      <c r="E54">
+        <v>4583285</v>
+      </c>
+      <c r="F54" t="s">
+        <v>225</v>
+      </c>
+      <c r="G54" t="s">
+        <v>208</v>
+      </c>
+      <c r="H54" s="49">
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>3276432</v>
+      </c>
+      <c r="B55" t="s">
+        <v>226</v>
+      </c>
+      <c r="C55" t="s">
+        <v>227</v>
+      </c>
+      <c r="D55" t="s">
+        <v>228</v>
+      </c>
+      <c r="E55">
+        <v>3364439</v>
+      </c>
+      <c r="F55" t="s">
+        <v>229</v>
+      </c>
+      <c r="G55" t="s">
+        <v>208</v>
+      </c>
+      <c r="H55" s="49">
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>3274543</v>
+      </c>
+      <c r="B56" t="s">
+        <v>176</v>
+      </c>
+      <c r="C56" t="s">
+        <v>165</v>
+      </c>
+      <c r="D56" t="s">
+        <v>177</v>
+      </c>
+      <c r="F56" t="s">
+        <v>178</v>
+      </c>
+      <c r="G56" t="s">
+        <v>106</v>
+      </c>
+      <c r="H56" s="49">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -2846,18 +3200,18 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.453125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="17.81640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.81640625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="25.26953125" style="10" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" style="12" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11">
         <v>2663720</v>
       </c>
@@ -2883,7 +3237,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -2891,7 +3245,7 @@
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>3037547</v>
       </c>
@@ -2920,7 +3274,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -2928,7 +3282,7 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>3067160</v>
       </c>
@@ -2954,7 +3308,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -2962,7 +3316,7 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>3265971</v>
       </c>
@@ -2986,7 +3340,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>3266023</v>
       </c>
@@ -3010,7 +3364,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -3018,7 +3372,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>2949099</v>
       </c>
@@ -3044,7 +3398,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
@@ -3052,7 +3406,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>2652454</v>
       </c>
@@ -3078,7 +3432,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -3086,7 +3440,7 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>3266321</v>
       </c>
@@ -3116,7 +3470,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>3265990</v>
       </c>
@@ -3140,7 +3494,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
@@ -3148,7 +3502,7 @@
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
     </row>
-    <row r="17" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>3073191</v>
       </c>
@@ -3180,7 +3534,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
@@ -3188,7 +3542,7 @@
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
     </row>
-    <row r="19" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>3266265</v>
       </c>
@@ -3212,7 +3566,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
         <v>3266180</v>
       </c>
@@ -3236,7 +3590,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -3244,7 +3598,7 @@
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
     </row>
-    <row r="22" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>3266324</v>
       </c>
@@ -3270,7 +3624,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
@@ -3278,7 +3632,7 @@
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
     </row>
-    <row r="24" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>78</v>
       </c>
@@ -3298,7 +3652,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -3306,7 +3660,7 @@
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
     </row>
-    <row r="26" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <v>3266106</v>
       </c>
@@ -3346,19 +3700,19 @@
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.54296875" style="12" customWidth="1"/>
-    <col min="2" max="2" width="22.26953125" style="12" customWidth="1"/>
-    <col min="3" max="3" width="6.54296875" style="12" customWidth="1"/>
-    <col min="4" max="4" width="26.7265625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="45" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="44" t="s">
         <v>127</v>
       </c>
       <c r="C1" s="11" t="s">
@@ -3376,9 +3730,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="39"/>
-      <c r="B2" s="38"/>
+    <row r="2" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="45"/>
+      <c r="B2" s="44"/>
       <c r="C2" s="11" t="s">
         <v>126</v>
       </c>
@@ -3388,7 +3742,7 @@
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>79</v>
       </c>
@@ -3408,7 +3762,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -3416,7 +3770,7 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>3266133</v>
       </c>
@@ -3440,7 +3794,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -3448,7 +3802,7 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>84</v>
       </c>
@@ -3468,7 +3822,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>86</v>
       </c>
@@ -3488,7 +3842,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -3496,7 +3850,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>2955619</v>
       </c>
@@ -3522,7 +3876,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
@@ -3530,7 +3884,7 @@
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>3266289</v>
       </c>
@@ -3559,7 +3913,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -3567,7 +3921,7 @@
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>2657085</v>
       </c>
@@ -3593,7 +3947,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -3601,7 +3955,7 @@
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>3037067</v>
       </c>
@@ -3633,7 +3987,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -3641,7 +3995,7 @@
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
     </row>
-    <row r="18" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>89</v>
       </c>
@@ -3661,7 +4015,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -3669,7 +4023,7 @@
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
     </row>
-    <row r="20" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
         <v>2958822</v>
       </c>
@@ -3701,7 +4055,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -3709,7 +4063,7 @@
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
     </row>
-    <row r="22" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>2951874</v>
       </c>
@@ -3735,7 +4089,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
         <v>2966414</v>
       </c>
@@ -3761,7 +4115,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
@@ -3769,7 +4123,7 @@
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
     </row>
-    <row r="25" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>116</v>
       </c>
@@ -3788,7 +4142,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="17" t="s">
         <v>122</v>
@@ -3808,7 +4162,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -3816,7 +4170,7 @@
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
     </row>
-    <row r="28" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>130</v>
       </c>
@@ -3827,13 +4181,13 @@
       <c r="D28" s="9"/>
       <c r="F28" s="7"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B32"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34"/>
     </row>
   </sheetData>
@@ -3848,26 +4202,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A13:XFD29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33" style="41" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" customWidth="1"/>
-    <col min="6" max="6" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33" style="38" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7">
         <v>2966808</v>
       </c>
@@ -3877,7 +4231,7 @@
       <c r="C1" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="43" t="s">
         <v>166</v>
       </c>
       <c r="E1" s="7">
@@ -3893,15 +4247,15 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
-      <c r="D2" s="43"/>
+      <c r="D2" s="40"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>3274543</v>
       </c>
@@ -3911,7 +4265,7 @@
       <c r="C3" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="39" t="s">
         <v>177</v>
       </c>
       <c r="E3" s="7"/>
@@ -3925,15 +4279,15 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
-      <c r="D4" s="43"/>
+      <c r="D4" s="40"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>3274419</v>
       </c>
@@ -3943,7 +4297,7 @@
       <c r="C5" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="39" t="s">
         <v>170</v>
       </c>
       <c r="E5" s="7"/>
@@ -3957,15 +4311,15 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
-      <c r="D6" s="43"/>
+      <c r="D6" s="40"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>3274740</v>
       </c>
@@ -3975,7 +4329,7 @@
       <c r="C7" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="D7" s="42" t="s">
+      <c r="D7" s="39" t="s">
         <v>156</v>
       </c>
       <c r="E7" s="7"/>
@@ -3989,15 +4343,15 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
-      <c r="D8" s="43"/>
+      <c r="D8" s="40"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>3274450</v>
       </c>
@@ -4007,7 +4361,7 @@
       <c r="C9" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="D9" s="42" t="s">
+      <c r="D9" s="39" t="s">
         <v>153</v>
       </c>
       <c r="E9" s="7"/>
@@ -4021,15 +4375,15 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
-      <c r="D10" s="43"/>
+      <c r="D10" s="40"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>3274597</v>
       </c>
@@ -4039,7 +4393,7 @@
       <c r="C11" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="D11" s="42" t="s">
+      <c r="D11" s="39" t="s">
         <v>174</v>
       </c>
       <c r="E11" s="7"/>
@@ -4053,24 +4407,274 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
-      <c r="D12" s="43"/>
+      <c r="D12" s="40"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="44" t="s">
+    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>2961585</v>
+      </c>
+      <c r="B35" t="s">
+        <v>158</v>
+      </c>
+      <c r="C35" t="s">
+        <v>159</v>
+      </c>
+      <c r="D35" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="E35" t="s">
+        <v>161</v>
+      </c>
+      <c r="F35" t="s">
+        <v>162</v>
+      </c>
+      <c r="G35" t="s">
+        <v>96</v>
+      </c>
+      <c r="H35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>2962452</v>
+      </c>
+      <c r="B36" t="s">
+        <v>158</v>
+      </c>
+      <c r="C36" t="s">
+        <v>159</v>
+      </c>
+      <c r="D36" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="E36" t="s">
+        <v>161</v>
+      </c>
+      <c r="F36" t="s">
+        <v>163</v>
+      </c>
+      <c r="G36" t="s">
+        <v>96</v>
+      </c>
+      <c r="H36">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="41" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" s="16"/>
+      <c r="F1" s="15"/>
+      <c r="G1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="41" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="E3" s="16"/>
+      <c r="F3" s="15"/>
+      <c r="G3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="41" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="E5" s="16"/>
+      <c r="F5" s="15"/>
+      <c r="G5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="50"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+    </row>
+    <row r="7" spans="1:9" s="56" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>3268531</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="E7" s="7">
+        <v>6484</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="G7" s="56" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="56" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="52" t="s">
         <v>134</v>
       </c>
-      <c r="B13" s="7"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="54" t="s">
+        <v>135</v>
+      </c>
+      <c r="D9" s="54" t="s">
+        <v>136</v>
+      </c>
+      <c r="E9" s="55"/>
+      <c r="F9" s="54"/>
+      <c r="G9" t="s">
+        <v>82</v>
+      </c>
+      <c r="H9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="41" t="s">
+        <v>193</v>
+      </c>
+      <c r="B11" s="42"/>
+      <c r="C11" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="E11" s="16"/>
+      <c r="F11" s="15"/>
+      <c r="G11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H11">
+        <v>35</v>
+      </c>
+      <c r="I11" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="B13" s="42" t="s">
+        <v>192</v>
+      </c>
       <c r="C13" s="15" t="s">
-        <v>149</v>
+        <v>190</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>150</v>
+        <v>191</v>
       </c>
       <c r="E13" s="16"/>
       <c r="F13" s="15"/>
@@ -4081,24 +4685,24 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
-      <c r="D14" s="43"/>
+      <c r="D14" s="40"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="44" t="s">
-        <v>148</v>
-      </c>
-      <c r="B15" s="45"/>
+    <row r="15" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="41" t="s">
+        <v>195</v>
+      </c>
+      <c r="B15" s="42"/>
       <c r="C15" s="15" t="s">
-        <v>146</v>
+        <v>188</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>147</v>
+        <v>189</v>
       </c>
       <c r="E15" s="16"/>
       <c r="F15" s="15"/>
@@ -4109,24 +4713,24 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
-      <c r="D16" s="43"/>
+      <c r="D16" s="40"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
     </row>
-    <row r="17" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="44" t="s">
-        <v>195</v>
-      </c>
-      <c r="B17" s="45"/>
+    <row r="17" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="41" t="s">
+        <v>148</v>
+      </c>
+      <c r="B17" s="42"/>
       <c r="C17" s="15" t="s">
-        <v>188</v>
+        <v>146</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>189</v>
+        <v>147</v>
       </c>
       <c r="E17" s="16"/>
       <c r="F17" s="15"/>
@@ -4137,24 +4741,24 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
-      <c r="D18" s="43"/>
+      <c r="D18" s="40"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
     </row>
-    <row r="19" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="44" t="s">
-        <v>193</v>
-      </c>
-      <c r="B19" s="45"/>
+    <row r="19" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="41" t="s">
+        <v>134</v>
+      </c>
+      <c r="B19" s="7"/>
       <c r="C19" s="15" t="s">
-        <v>190</v>
+        <v>149</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>191</v>
+        <v>150</v>
       </c>
       <c r="E19" s="16"/>
       <c r="F19" s="15"/>
@@ -4164,206 +4768,48 @@
       <c r="H19">
         <v>35</v>
       </c>
-      <c r="I19" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
-      <c r="D20" s="43"/>
+      <c r="D20" s="40"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
     </row>
-    <row r="21" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="44" t="s">
-        <v>194</v>
-      </c>
-      <c r="B21" s="45" t="s">
-        <v>192</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="E21" s="16"/>
-      <c r="F21" s="15"/>
+    <row r="21" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>3268534</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="E21" s="7">
+        <v>1862974</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>216</v>
+      </c>
       <c r="G21" t="s">
-        <v>82</v>
-      </c>
-      <c r="H21">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
-      <c r="D22" s="43"/>
+      <c r="D22" s="7"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
     </row>
-    <row r="23" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="44" t="s">
-        <v>134</v>
-      </c>
-      <c r="B23" s="45"/>
-      <c r="C23" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="E23" s="16"/>
-      <c r="F23" s="15"/>
-      <c r="G23" t="s">
-        <v>82</v>
-      </c>
-      <c r="H23">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-    </row>
-    <row r="25" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="44" t="s">
-        <v>142</v>
-      </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="E25" s="16"/>
-      <c r="F25" s="15"/>
-      <c r="G25" t="s">
-        <v>82</v>
-      </c>
-      <c r="H25">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-    </row>
-    <row r="27" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="44" t="s">
-        <v>145</v>
-      </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="E27" s="16"/>
-      <c r="F27" s="15"/>
-      <c r="G27" t="s">
-        <v>82</v>
-      </c>
-      <c r="H27">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-    </row>
-    <row r="29" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="44" t="s">
-        <v>139</v>
-      </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="E29" s="16"/>
-      <c r="F29" s="15"/>
-      <c r="G29" t="s">
-        <v>82</v>
-      </c>
-      <c r="H29">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35">
-        <v>2961585</v>
-      </c>
-      <c r="B35" t="s">
-        <v>158</v>
-      </c>
-      <c r="C35" t="s">
-        <v>159</v>
-      </c>
-      <c r="D35" s="40" t="s">
-        <v>160</v>
-      </c>
-      <c r="E35" t="s">
-        <v>161</v>
-      </c>
-      <c r="F35" t="s">
-        <v>162</v>
-      </c>
-      <c r="G35" t="s">
-        <v>96</v>
-      </c>
-      <c r="H35">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36">
-        <v>2962452</v>
-      </c>
-      <c r="B36" t="s">
-        <v>158</v>
-      </c>
-      <c r="C36" t="s">
-        <v>159</v>
-      </c>
-      <c r="D36" s="40" t="s">
-        <v>160</v>
-      </c>
-      <c r="E36" t="s">
-        <v>161</v>
-      </c>
-      <c r="F36" t="s">
-        <v>163</v>
-      </c>
-      <c r="G36" t="s">
-        <v>96</v>
-      </c>
-      <c r="H36">
-        <v>70</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>